<commit_message>
Mise à jour des données au 8 janvier 2018
</commit_message>
<xml_diff>
--- a/raw/Individu.xlsx
+++ b/raw/Individu.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="658">
   <si>
     <t>Bac ou équivalence (code)</t>
   </si>
@@ -1902,12 +1902,6 @@
   </si>
   <si>
     <t>GRENADE ETGRENADINES</t>
-  </si>
-  <si>
-    <t>436</t>
-  </si>
-  <si>
-    <t>BAHAMAS</t>
   </si>
   <si>
     <t>437</t>
@@ -5317,7 +5311,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C184"/>
+  <dimension ref="A1:C183"/>
   <cols>
     <col min="1" max="1" width="30.2315986666667" customWidth="1"/>
     <col min="2" max="2" width="10.7163133333333" customWidth="1"/>
@@ -6667,15 +6661,15 @@
         <v>632</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>633</v>
+        <v>591</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="1" ht="19.7321" customHeight="1">
       <c r="B170" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="C170" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="C170" s="4" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="1" ht="19.7321" customHeight="1">
@@ -6771,18 +6765,10 @@
         <v>657</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="183" s="1" customFormat="1" ht="19.7321" customHeight="1">
-      <c r="B183" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="C183" s="3" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="184" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="183" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>